<commit_message>
removing lists from eb09-s01
</commit_message>
<xml_diff>
--- a/page/eb09/s01/eb09-s01.xlsx
+++ b/page/eb09/s01/eb09-s01.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\knowledge-project\kp2\page\eb09\s01\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D2C7E2-B8F0-4DC6-95C5-EA69E829B5EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="2685" windowWidth="21735" windowHeight="12090"/>
+    <workbookView xWindow="-28650" yWindow="180" windowWidth="13965" windowHeight="17565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eb09-s01" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="551">
   <si>
     <t>eb09-s01</t>
   </si>
@@ -1655,9 +1656,6 @@
     <t xml:space="preserve">Sanskrit; double reference to footnote #2: </t>
   </si>
   <si>
-    <t>list runs over to next page</t>
-  </si>
-  <si>
     <t>tables need correction</t>
   </si>
   <si>
@@ -1677,12 +1675,15 @@
   </si>
   <si>
     <t>removed &lt;list&gt;</t>
+  </si>
+  <si>
+    <t>fixed tables; removed &lt;list&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -2054,11 +2055,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L257"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
-      <selection activeCell="L105" sqref="L105:L106"/>
+    <sheetView tabSelected="1" topLeftCell="B136" workbookViewId="0">
+      <selection activeCell="L148" sqref="L147:L148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2066,13 +2067,15 @@
     <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="12" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="22.5703125" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2816,7 +2819,7 @@
         <v>533</v>
       </c>
       <c r="L35" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -3416,7 +3419,7 @@
       <c r="I65" s="8"/>
       <c r="K65" s="3"/>
       <c r="L65" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -3499,7 +3502,7 @@
       <c r="I69" s="8"/>
       <c r="K69" s="3"/>
       <c r="L69" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -4148,7 +4151,7 @@
       <c r="I99" s="8"/>
       <c r="K99" s="3"/>
       <c r="L99" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -4172,7 +4175,7 @@
       <c r="I100" s="8"/>
       <c r="K100" s="3"/>
       <c r="L100" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -4280,7 +4283,7 @@
       <c r="I105" s="8"/>
       <c r="K105" s="3"/>
       <c r="L105" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
@@ -4304,7 +4307,7 @@
       <c r="I106" s="8"/>
       <c r="K106" s="3"/>
       <c r="L106" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
@@ -4328,7 +4331,7 @@
       <c r="I107" s="8"/>
       <c r="K107" s="3"/>
       <c r="L107" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
@@ -4352,7 +4355,7 @@
       <c r="I108" s="8"/>
       <c r="K108" s="3"/>
       <c r="L108" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
@@ -4439,7 +4442,7 @@
       <c r="I112" s="8"/>
       <c r="K112" s="3"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3" t="s">
         <v>232</v>
@@ -4460,7 +4463,7 @@
       <c r="I113" s="8"/>
       <c r="K113" s="3"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="3" t="s">
         <v>234</v>
@@ -4481,7 +4484,7 @@
       <c r="I114" s="8"/>
       <c r="K114" s="3"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="3" t="s">
         <v>236</v>
@@ -4502,7 +4505,7 @@
       <c r="I115" s="8"/>
       <c r="K115" s="3"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="3" t="s">
         <v>238</v>
@@ -4523,7 +4526,7 @@
       <c r="I116" s="8"/>
       <c r="K116" s="3"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="3" t="s">
         <v>240</v>
@@ -4544,7 +4547,7 @@
       <c r="I117" s="8"/>
       <c r="K117" s="3"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="3" t="s">
         <v>242</v>
@@ -4565,10 +4568,13 @@
       <c r="I118" s="8"/>
       <c r="K118" s="3"/>
       <c r="L118" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="M118" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="3" t="s">
         <v>244</v>
@@ -4589,7 +4595,7 @@
       <c r="I119" s="8"/>
       <c r="K119" s="3"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="3" t="s">
         <v>246</v>
@@ -4610,7 +4616,7 @@
       <c r="I120" s="8"/>
       <c r="K120" s="3"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="3" t="s">
         <v>248</v>
@@ -4633,7 +4639,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="3" t="s">
         <v>251</v>
@@ -4654,7 +4660,7 @@
       <c r="I122" s="8"/>
       <c r="K122" s="3"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3" t="s">
         <v>253</v>
@@ -4675,7 +4681,7 @@
       <c r="I123" s="8"/>
       <c r="K123" s="3"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3" t="s">
         <v>255</v>
@@ -4696,7 +4702,7 @@
       <c r="I124" s="8"/>
       <c r="K124" s="3"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="3" t="s">
         <v>257</v>
@@ -4717,7 +4723,7 @@
       <c r="I125" s="8"/>
       <c r="K125" s="3"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3" t="s">
         <v>259</v>
@@ -4738,7 +4744,7 @@
       <c r="I126" s="8"/>
       <c r="K126" s="3"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3" t="s">
         <v>261</v>
@@ -4761,7 +4767,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3" t="s">
         <v>263</v>
@@ -4782,7 +4788,7 @@
       <c r="I128" s="8"/>
       <c r="K128" s="3"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3" t="s">
         <v>265</v>
@@ -4803,7 +4809,7 @@
       <c r="I129" s="8"/>
       <c r="K129" s="3"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3" t="s">
         <v>267</v>
@@ -4824,7 +4830,7 @@
       <c r="I130" s="8"/>
       <c r="K130" s="3"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="3" t="s">
         <v>269</v>
@@ -4845,7 +4851,7 @@
       <c r="I131" s="8"/>
       <c r="K131" s="3"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3" t="s">
         <v>271</v>
@@ -4866,7 +4872,7 @@
       <c r="I132" s="8"/>
       <c r="K132" s="3"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="3" t="s">
         <v>273</v>
@@ -4887,7 +4893,7 @@
       <c r="I133" s="8"/>
       <c r="K133" s="3"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="3" t="s">
         <v>275</v>
@@ -4908,7 +4914,7 @@
       <c r="I134" s="8"/>
       <c r="K134" s="3"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="3" t="s">
         <v>277</v>
@@ -4929,7 +4935,7 @@
       <c r="I135" s="8"/>
       <c r="K135" s="3"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="3" t="s">
         <v>279</v>
@@ -4952,7 +4958,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="3" t="s">
         <v>281</v>
@@ -4972,8 +4978,11 @@
       </c>
       <c r="I137" s="8"/>
       <c r="K137" s="3"/>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M137" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="3" t="s">
         <v>283</v>
@@ -4994,7 +5003,7 @@
       <c r="I138" s="8"/>
       <c r="K138" s="3"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="3" t="s">
         <v>285</v>
@@ -5017,7 +5026,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="3" t="s">
         <v>287</v>
@@ -5038,7 +5047,7 @@
       <c r="I140" s="8"/>
       <c r="K140" s="3"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="3" t="s">
         <v>289</v>
@@ -5059,7 +5068,7 @@
       <c r="I141" s="8"/>
       <c r="K141" s="3"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="3" t="s">
         <v>291</v>
@@ -5080,7 +5089,7 @@
       <c r="I142" s="8"/>
       <c r="K142" s="3"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="3" t="s">
         <v>293</v>
@@ -5101,7 +5110,7 @@
       <c r="I143" s="8"/>
       <c r="K143" s="3"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="3" t="s">
         <v>295</v>
@@ -5122,7 +5131,7 @@
       <c r="I144" s="8"/>
       <c r="K144" s="3"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="3" t="s">
         <v>297</v>
@@ -5143,7 +5152,7 @@
       <c r="I145" s="8"/>
       <c r="K145" s="3"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="3" t="s">
         <v>299</v>
@@ -5164,7 +5173,7 @@
       <c r="I146" s="8"/>
       <c r="K146" s="3"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="3" t="s">
         <v>301</v>
@@ -5185,7 +5194,7 @@
       <c r="I147" s="8"/>
       <c r="K147" s="3"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="3" t="s">
         <v>303</v>
@@ -5206,7 +5215,7 @@
       <c r="I148" s="8"/>
       <c r="K148" s="3"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="3" t="s">
         <v>305</v>
@@ -5226,8 +5235,11 @@
       </c>
       <c r="I149" s="8"/>
       <c r="K149" s="3"/>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M149" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="3" t="s">
         <v>307</v>
@@ -5248,7 +5260,7 @@
       <c r="I150" s="8"/>
       <c r="K150" s="3"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="3" t="s">
         <v>309</v>
@@ -5269,7 +5281,7 @@
       <c r="I151" s="8"/>
       <c r="K151" s="3"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="3" t="s">
         <v>311</v>
@@ -5290,7 +5302,7 @@
       <c r="I152" s="8"/>
       <c r="K152" s="3"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="3" t="s">
         <v>313</v>
@@ -5313,7 +5325,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="3" t="s">
         <v>316</v>
@@ -5335,8 +5347,11 @@
       <c r="K154" s="3" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M154" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="3" t="s">
         <v>318</v>
@@ -5359,7 +5374,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="3" t="s">
         <v>320</v>
@@ -5382,7 +5397,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
       <c r="B157" s="3" t="s">
         <v>322</v>
@@ -5405,7 +5420,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
       <c r="B158" s="3" t="s">
         <v>324</v>
@@ -5428,7 +5443,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
       <c r="B159" s="3" t="s">
         <v>326</v>
@@ -5451,7 +5466,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
       <c r="B160" s="3" t="s">
         <v>328</v>
@@ -5825,7 +5840,7 @@
         <v>542</v>
       </c>
       <c r="L175" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.25">
@@ -7501,7 +7516,7 @@
         <v>517</v>
       </c>
       <c r="L254" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>